<commit_message>
Add faker to distributions
</commit_message>
<xml_diff>
--- a/data/distributions.xlsx
+++ b/data/distributions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1540" yWindow="4980" windowWidth="21340" windowHeight="11980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all branch segments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
   <si>
     <t>repository</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>docker</t>
+  </si>
+  <si>
+    <t>faker</t>
   </si>
 </sst>
 </file>
@@ -307,9 +310,179 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="364">
+  <cellStyleXfs count="534">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -678,7 +851,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="364">
+  <cellStyles count="534">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -860,6 +1033,91 @@
     <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="431" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="433" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="435" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="437" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="439" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="499" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="501" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="503" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="505" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="507" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="509" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="511" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="513" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1041,6 +1299,91 @@
     <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="430" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="432" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="434" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="436" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="438" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="440" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="442" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="444" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="446" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="498" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="500" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="502" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="504" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="506" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="508" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="510" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="512" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1371,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL6"/>
+  <dimension ref="A1:BL7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2609,6 +2952,200 @@
         <v>213.75988326999999</v>
       </c>
     </row>
+    <row r="7" spans="1:64">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <v>2.3971830985999998</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2.8616878898999998</v>
+      </c>
+      <c r="E7">
+        <v>3.7267605634000001</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>7.7831659161999998</v>
+      </c>
+      <c r="H7">
+        <v>2.1631434626999999</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>6.6928603545999996</v>
+      </c>
+      <c r="K7">
+        <v>3.9915492958000001</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>8.3755385437999994</v>
+      </c>
+      <c r="N7">
+        <v>2.2088261236000002</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>6.7117858732000002</v>
+      </c>
+      <c r="Q7">
+        <v>276.85352112999999</v>
+      </c>
+      <c r="R7">
+        <v>21</v>
+      </c>
+      <c r="S7">
+        <v>1246.4288313</v>
+      </c>
+      <c r="T7">
+        <v>73.802816901</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>811.80551405000006</v>
+      </c>
+      <c r="W7">
+        <v>350.65633802999997</v>
+      </c>
+      <c r="X7">
+        <v>31</v>
+      </c>
+      <c r="Y7">
+        <v>1650.1030443</v>
+      </c>
+      <c r="Z7">
+        <v>213.26967146999999</v>
+      </c>
+      <c r="AA7">
+        <v>15.052631579</v>
+      </c>
+      <c r="AB7">
+        <v>1438.1492714000001</v>
+      </c>
+      <c r="AC7">
+        <v>332.57464788999999</v>
+      </c>
+      <c r="AD7">
+        <v>24</v>
+      </c>
+      <c r="AE7">
+        <v>1368.7708276000001</v>
+      </c>
+      <c r="AF7">
+        <v>129.52394365999999</v>
+      </c>
+      <c r="AG7">
+        <v>3</v>
+      </c>
+      <c r="AH7">
+        <v>923.19778402999998</v>
+      </c>
+      <c r="AI7">
+        <v>462.09859154999998</v>
+      </c>
+      <c r="AJ7">
+        <v>38</v>
+      </c>
+      <c r="AK7">
+        <v>1936.3030398000001</v>
+      </c>
+      <c r="AL7">
+        <v>243.15153477999999</v>
+      </c>
+      <c r="AM7">
+        <v>19</v>
+      </c>
+      <c r="AN7">
+        <v>1495.6615693000001</v>
+      </c>
+      <c r="AO7">
+        <v>8.4563380281999994</v>
+      </c>
+      <c r="AP7">
+        <v>3</v>
+      </c>
+      <c r="AQ7">
+        <v>27.396238412999999</v>
+      </c>
+      <c r="AR7">
+        <v>5.5189169927000004</v>
+      </c>
+      <c r="AS7">
+        <v>1.2857142856999999</v>
+      </c>
+      <c r="AT7">
+        <v>25.32042994</v>
+      </c>
+      <c r="AU7">
+        <v>13.856338028</v>
+      </c>
+      <c r="AV7">
+        <v>4</v>
+      </c>
+      <c r="AW7">
+        <v>35.675628787000001</v>
+      </c>
+      <c r="AX7">
+        <v>6.4982508773000003</v>
+      </c>
+      <c r="AY7">
+        <v>2.25</v>
+      </c>
+      <c r="AZ7">
+        <v>25.313301603999999</v>
+      </c>
+      <c r="BA7">
+        <v>1.0281690140999999</v>
+      </c>
+      <c r="BB7">
+        <v>1</v>
+      </c>
+      <c r="BC7">
+        <v>0.1656890241</v>
+      </c>
+      <c r="BD7">
+        <v>1.0084507041999999</v>
+      </c>
+      <c r="BE7">
+        <v>1</v>
+      </c>
+      <c r="BF7">
+        <v>9.1667661299999995E-2</v>
+      </c>
+      <c r="BG7">
+        <v>72.174296557000005</v>
+      </c>
+      <c r="BH7">
+        <v>0</v>
+      </c>
+      <c r="BI7">
+        <v>325.6367856</v>
+      </c>
+      <c r="BJ7">
+        <v>140.04876213</v>
+      </c>
+      <c r="BK7">
+        <v>0</v>
+      </c>
+      <c r="BL7">
+        <v>560.25200443000006</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2622,10 +3159,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR6"/>
+  <dimension ref="A1:BR7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3781,9 +4318,427 @@
       <c r="B6">
         <v>5317</v>
       </c>
+      <c r="C6">
+        <v>9225</v>
+      </c>
       <c r="D6">
         <f>B6-4034</f>
         <v>1283</v>
+      </c>
+      <c r="E6">
+        <v>5191</v>
+      </c>
+      <c r="F6" s="1">
+        <f>D6/B6</f>
+        <v>0.24130148580026331</v>
+      </c>
+      <c r="G6" s="1">
+        <f>E6/C6</f>
+        <v>0.56271002710027096</v>
+      </c>
+      <c r="H6">
+        <v>4.0459860000000001</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>6.4188372999999999</v>
+      </c>
+      <c r="K6">
+        <v>7.4528448999999997</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>16.843686000000002</v>
+      </c>
+      <c r="N6">
+        <v>2.2357828</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>5.8824123999999998</v>
+      </c>
+      <c r="Q6">
+        <v>7.6017146999999996</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>16.975376000000001</v>
+      </c>
+      <c r="T6">
+        <v>2.2658214000000001</v>
+      </c>
+      <c r="U6">
+        <v>1.0793699999999999</v>
+      </c>
+      <c r="V6">
+        <v>5.8919566000000003</v>
+      </c>
+      <c r="W6">
+        <v>286.06391000000002</v>
+      </c>
+      <c r="X6">
+        <v>52</v>
+      </c>
+      <c r="Y6">
+        <v>2437.5228000000002</v>
+      </c>
+      <c r="Z6">
+        <v>137.31177</v>
+      </c>
+      <c r="AA6">
+        <v>14</v>
+      </c>
+      <c r="AB6">
+        <v>1344.1079</v>
+      </c>
+      <c r="AC6">
+        <v>423.37567999999999</v>
+      </c>
+      <c r="AD6">
+        <v>74</v>
+      </c>
+      <c r="AE6">
+        <v>2819.3766999999998</v>
+      </c>
+      <c r="AF6">
+        <v>130.04085000000001</v>
+      </c>
+      <c r="AG6">
+        <v>26.5</v>
+      </c>
+      <c r="AH6">
+        <v>1243.2153000000001</v>
+      </c>
+      <c r="AI6">
+        <v>308.45985999999999</v>
+      </c>
+      <c r="AJ6">
+        <v>56</v>
+      </c>
+      <c r="AK6">
+        <v>2447.6952999999999</v>
+      </c>
+      <c r="AL6">
+        <v>159.70771999999999</v>
+      </c>
+      <c r="AM6">
+        <v>19</v>
+      </c>
+      <c r="AN6">
+        <v>1350.6339</v>
+      </c>
+      <c r="AO6">
+        <v>468.16757999999999</v>
+      </c>
+      <c r="AP6">
+        <v>82</v>
+      </c>
+      <c r="AQ6">
+        <v>2843.1401999999998</v>
+      </c>
+      <c r="AR6">
+        <v>136.82284999999999</v>
+      </c>
+      <c r="AS6">
+        <v>30.5</v>
+      </c>
+      <c r="AT6">
+        <v>1243.7831000000001</v>
+      </c>
+      <c r="AU6">
+        <v>28.440373999999998</v>
+      </c>
+      <c r="AV6">
+        <v>10</v>
+      </c>
+      <c r="AW6">
+        <v>79.173432000000005</v>
+      </c>
+      <c r="AX6">
+        <v>8.3636347000000004</v>
+      </c>
+      <c r="AY6">
+        <v>3.5</v>
+      </c>
+      <c r="AZ6">
+        <v>32.841797999999997</v>
+      </c>
+      <c r="BA6">
+        <v>38.102884000000003</v>
+      </c>
+      <c r="BB6">
+        <v>13</v>
+      </c>
+      <c r="BC6">
+        <v>93.837108000000001</v>
+      </c>
+      <c r="BD6">
+        <v>10.004082</v>
+      </c>
+      <c r="BE6">
+        <v>4.5</v>
+      </c>
+      <c r="BF6">
+        <v>34.174511000000003</v>
+      </c>
+      <c r="BG6">
+        <v>1.3546376</v>
+      </c>
+      <c r="BH6">
+        <v>1</v>
+      </c>
+      <c r="BI6">
+        <v>2.0385596000000001</v>
+      </c>
+      <c r="BJ6">
+        <v>1.0623539</v>
+      </c>
+      <c r="BK6">
+        <v>1</v>
+      </c>
+      <c r="BL6">
+        <v>0.25446360000000001</v>
+      </c>
+      <c r="BM6">
+        <v>22.329066999999998</v>
+      </c>
+      <c r="BN6">
+        <v>0.74167000000000005</v>
+      </c>
+      <c r="BO6">
+        <v>72.947642999999999</v>
+      </c>
+      <c r="BP6">
+        <v>148.30341000000001</v>
+      </c>
+      <c r="BQ6">
+        <v>13.6492</v>
+      </c>
+      <c r="BR6">
+        <v>415.66107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:70">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <v>365</v>
+      </c>
+      <c r="C7">
+        <v>851</v>
+      </c>
+      <c r="D7">
+        <f>B7-196</f>
+        <v>169</v>
+      </c>
+      <c r="E7">
+        <v>655</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ref="F7:F18" si="0">D7/B7</f>
+        <v>0.46301369863013697</v>
+      </c>
+      <c r="G7" s="1">
+        <f>E7/C7</f>
+        <v>0.76968272620446532</v>
+      </c>
+      <c r="H7">
+        <v>4.1194968999999997</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>3.5974054999999998</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>6.1170026999999996</v>
+      </c>
+      <c r="N7">
+        <v>1.5089052000000001</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>2.0566537999999999</v>
+      </c>
+      <c r="Q7">
+        <v>5.5911949999999999</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>7.5600664999999996</v>
+      </c>
+      <c r="T7">
+        <v>1.6109011</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>2.2196267000000001</v>
+      </c>
+      <c r="W7">
+        <v>400.06288999999998</v>
+      </c>
+      <c r="X7">
+        <v>93</v>
+      </c>
+      <c r="Y7">
+        <v>1281.9567</v>
+      </c>
+      <c r="Z7">
+        <v>42.918239</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>157.84125</v>
+      </c>
+      <c r="AC7">
+        <v>442.98113000000001</v>
+      </c>
+      <c r="AD7">
+        <v>110</v>
+      </c>
+      <c r="AE7">
+        <v>1298.4916000000001</v>
+      </c>
+      <c r="AF7">
+        <v>136.23732000000001</v>
+      </c>
+      <c r="AG7">
+        <v>31.2</v>
+      </c>
+      <c r="AH7">
+        <v>473.54007000000001</v>
+      </c>
+      <c r="AI7">
+        <v>524.47170000000006</v>
+      </c>
+      <c r="AJ7">
+        <v>123</v>
+      </c>
+      <c r="AK7">
+        <v>1523.4204999999999</v>
+      </c>
+      <c r="AL7">
+        <v>167.32704000000001</v>
+      </c>
+      <c r="AM7">
+        <v>14</v>
+      </c>
+      <c r="AN7">
+        <v>676.06308000000001</v>
+      </c>
+      <c r="AO7">
+        <v>691.79873999999995</v>
+      </c>
+      <c r="AP7">
+        <v>152</v>
+      </c>
+      <c r="AQ7">
+        <v>1976.1502</v>
+      </c>
+      <c r="AR7">
+        <v>202.95468</v>
+      </c>
+      <c r="AS7">
+        <v>42</v>
+      </c>
+      <c r="AT7">
+        <v>781.12228000000005</v>
+      </c>
+      <c r="AU7">
+        <v>9.7421384</v>
+      </c>
+      <c r="AV7">
+        <v>4</v>
+      </c>
+      <c r="AW7">
+        <v>17.633474</v>
+      </c>
+      <c r="AX7">
+        <v>3.1837455000000001</v>
+      </c>
+      <c r="AY7">
+        <v>1.3333299999999999</v>
+      </c>
+      <c r="AZ7">
+        <v>7.6704445000000003</v>
+      </c>
+      <c r="BA7">
+        <v>21.798742000000001</v>
+      </c>
+      <c r="BB7">
+        <v>11</v>
+      </c>
+      <c r="BC7">
+        <v>36.999448999999998</v>
+      </c>
+      <c r="BD7">
+        <v>5.3703086000000004</v>
+      </c>
+      <c r="BE7">
+        <v>3.3</v>
+      </c>
+      <c r="BF7">
+        <v>8.1023013000000006</v>
+      </c>
+      <c r="BG7">
+        <v>1.0628930999999999</v>
+      </c>
+      <c r="BH7">
+        <v>1</v>
+      </c>
+      <c r="BI7">
+        <v>0.24353759999999999</v>
+      </c>
+      <c r="BJ7">
+        <v>1.0188679</v>
+      </c>
+      <c r="BK7">
+        <v>1</v>
+      </c>
+      <c r="BL7">
+        <v>0.13648840000000001</v>
+      </c>
+      <c r="BM7">
+        <v>161.14386999999999</v>
+      </c>
+      <c r="BN7">
+        <v>3.3822199999999998</v>
+      </c>
+      <c r="BO7">
+        <v>472.39191</v>
+      </c>
+      <c r="BP7">
+        <v>312.68749000000003</v>
+      </c>
+      <c r="BQ7">
+        <v>16.827500000000001</v>
+      </c>
+      <c r="BR7">
+        <v>805.56295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add git to distributions
</commit_message>
<xml_diff>
--- a/data/distributions.xlsx
+++ b/data/distributions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="4980" windowWidth="21340" windowHeight="11980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="160" yWindow="5180" windowWidth="21340" windowHeight="11880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="all branch segments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
   <si>
     <t>repository</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>faker</t>
+  </si>
+  <si>
+    <t>git</t>
   </si>
 </sst>
 </file>
@@ -310,9 +313,93 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="534">
+  <cellStyleXfs count="618">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -851,7 +938,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="534">
+  <cellStyles count="618">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1118,6 +1205,48 @@
     <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1384,6 +1513,48 @@
     <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1714,10 +1885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL7"/>
+  <dimension ref="A1:BL8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3146,6 +3317,200 @@
         <v>560.25200443000006</v>
       </c>
     </row>
+    <row r="8" spans="1:64">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8">
+        <v>3.3768472906000002</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>11.374127195</v>
+      </c>
+      <c r="E8">
+        <v>4.5110301992000004</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>9.7064627256999998</v>
+      </c>
+      <c r="H8">
+        <v>1.7696330951000001</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>4.0132459881000004</v>
+      </c>
+      <c r="K8">
+        <v>4.5238809166999996</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>9.7520353179000008</v>
+      </c>
+      <c r="N8">
+        <v>1.7713881890000001</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>4.0132822012</v>
+      </c>
+      <c r="Q8">
+        <v>134.70625401999999</v>
+      </c>
+      <c r="R8">
+        <v>26</v>
+      </c>
+      <c r="S8">
+        <v>705.3084791</v>
+      </c>
+      <c r="T8">
+        <v>51.795459413000003</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+      <c r="V8">
+        <v>250.72357905000001</v>
+      </c>
+      <c r="W8">
+        <v>186.50171343</v>
+      </c>
+      <c r="X8">
+        <v>36</v>
+      </c>
+      <c r="Y8">
+        <v>848.93752258999996</v>
+      </c>
+      <c r="Z8">
+        <v>59.941029284000003</v>
+      </c>
+      <c r="AA8">
+        <v>19</v>
+      </c>
+      <c r="AB8">
+        <v>246.77768237000001</v>
+      </c>
+      <c r="AC8">
+        <v>154.80316984000001</v>
+      </c>
+      <c r="AD8">
+        <v>26</v>
+      </c>
+      <c r="AE8">
+        <v>1333.1241574000001</v>
+      </c>
+      <c r="AF8">
+        <v>71.892375240999996</v>
+      </c>
+      <c r="AG8">
+        <v>7</v>
+      </c>
+      <c r="AH8">
+        <v>1162.9505340000001</v>
+      </c>
+      <c r="AI8">
+        <v>226.69554507999999</v>
+      </c>
+      <c r="AJ8">
+        <v>37</v>
+      </c>
+      <c r="AK8">
+        <v>2420.6193664000002</v>
+      </c>
+      <c r="AL8">
+        <v>61.30184843</v>
+      </c>
+      <c r="AM8">
+        <v>19.875</v>
+      </c>
+      <c r="AN8">
+        <v>249.0308378</v>
+      </c>
+      <c r="AO8">
+        <v>28.223495395</v>
+      </c>
+      <c r="AP8">
+        <v>6</v>
+      </c>
+      <c r="AQ8">
+        <v>148.22690814000001</v>
+      </c>
+      <c r="AR8">
+        <v>11.953771774</v>
+      </c>
+      <c r="AS8">
+        <v>3</v>
+      </c>
+      <c r="AT8">
+        <v>80.120498069000007</v>
+      </c>
+      <c r="AU8">
+        <v>35.544549154000002</v>
+      </c>
+      <c r="AV8">
+        <v>6</v>
+      </c>
+      <c r="AW8">
+        <v>270.44755229999998</v>
+      </c>
+      <c r="AX8">
+        <v>12.460389075</v>
+      </c>
+      <c r="AY8">
+        <v>3.5</v>
+      </c>
+      <c r="AZ8">
+        <v>80.514722559999996</v>
+      </c>
+      <c r="BA8">
+        <v>1.5515099592999999</v>
+      </c>
+      <c r="BB8">
+        <v>1</v>
+      </c>
+      <c r="BC8">
+        <v>1.3602365662</v>
+      </c>
+      <c r="BD8">
+        <v>1.0126365389</v>
+      </c>
+      <c r="BE8">
+        <v>1</v>
+      </c>
+      <c r="BF8">
+        <v>0.13434073730000001</v>
+      </c>
+      <c r="BG8">
+        <v>46.619348123999998</v>
+      </c>
+      <c r="BH8">
+        <v>0</v>
+      </c>
+      <c r="BI8">
+        <v>630.91710981999995</v>
+      </c>
+      <c r="BJ8">
+        <v>126.32424484000001</v>
+      </c>
+      <c r="BK8">
+        <v>0</v>
+      </c>
+      <c r="BL8">
+        <v>1131.3163784000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3159,10 +3524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR7"/>
+  <dimension ref="A1:BR8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4741,6 +5106,221 @@
         <v>805.56295</v>
       </c>
     </row>
+    <row r="8" spans="1:70">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8">
+        <v>9338</v>
+      </c>
+      <c r="C8">
+        <v>31533</v>
+      </c>
+      <c r="D8">
+        <f>B8-4693</f>
+        <v>4645</v>
+      </c>
+      <c r="E8">
+        <v>26840</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.49742985650032129</v>
+      </c>
+      <c r="G8" s="1">
+        <f>E8/C8</f>
+        <v>0.85117178828528839</v>
+      </c>
+      <c r="H8">
+        <v>5.7782562000000004</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>15.767991</v>
+      </c>
+      <c r="K8">
+        <v>6.9844995000000001</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>12.232538</v>
+      </c>
+      <c r="N8">
+        <v>1.4733765000000001</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>2.1433053000000002</v>
+      </c>
+      <c r="Q8">
+        <v>7.0103337000000003</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>12.299989</v>
+      </c>
+      <c r="T8">
+        <v>1.4769048</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>2.1439278000000002</v>
+      </c>
+      <c r="W8">
+        <v>227.00388000000001</v>
+      </c>
+      <c r="X8">
+        <v>62</v>
+      </c>
+      <c r="Y8">
+        <v>972.96515999999997</v>
+      </c>
+      <c r="Z8">
+        <v>84.373305000000002</v>
+      </c>
+      <c r="AA8">
+        <v>18</v>
+      </c>
+      <c r="AB8">
+        <v>332.86081000000001</v>
+      </c>
+      <c r="AC8">
+        <v>311.37718000000001</v>
+      </c>
+      <c r="AD8">
+        <v>89</v>
+      </c>
+      <c r="AE8">
+        <v>1154.7445</v>
+      </c>
+      <c r="AF8">
+        <v>56.947972</v>
+      </c>
+      <c r="AG8">
+        <v>23.333300000000001</v>
+      </c>
+      <c r="AH8">
+        <v>194.67671999999999</v>
+      </c>
+      <c r="AI8">
+        <v>267.40537999999998</v>
+      </c>
+      <c r="AJ8">
+        <v>64</v>
+      </c>
+      <c r="AK8">
+        <v>1873.8741</v>
+      </c>
+      <c r="AL8">
+        <v>124.77481</v>
+      </c>
+      <c r="AM8">
+        <v>21</v>
+      </c>
+      <c r="AN8">
+        <v>1643.2081000000001</v>
+      </c>
+      <c r="AO8">
+        <v>392.18018999999998</v>
+      </c>
+      <c r="AP8">
+        <v>93</v>
+      </c>
+      <c r="AQ8">
+        <v>3411.9780000000001</v>
+      </c>
+      <c r="AR8">
+        <v>59.683672999999999</v>
+      </c>
+      <c r="AS8">
+        <v>24.8</v>
+      </c>
+      <c r="AT8">
+        <v>200.39385999999999</v>
+      </c>
+      <c r="AU8">
+        <v>41.981484999999999</v>
+      </c>
+      <c r="AV8">
+        <v>13</v>
+      </c>
+      <c r="AW8">
+        <v>183.5401</v>
+      </c>
+      <c r="AX8">
+        <v>9.2739118999999999</v>
+      </c>
+      <c r="AY8">
+        <v>3.5</v>
+      </c>
+      <c r="AZ8">
+        <v>52.739424999999997</v>
+      </c>
+      <c r="BA8">
+        <v>56.699247</v>
+      </c>
+      <c r="BB8">
+        <v>15</v>
+      </c>
+      <c r="BC8">
+        <v>368.85532999999998</v>
+      </c>
+      <c r="BD8">
+        <v>10.292382</v>
+      </c>
+      <c r="BE8">
+        <v>4</v>
+      </c>
+      <c r="BF8">
+        <v>53.978757000000002</v>
+      </c>
+      <c r="BG8">
+        <v>2.1087191000000001</v>
+      </c>
+      <c r="BH8">
+        <v>2</v>
+      </c>
+      <c r="BI8">
+        <v>1.7612745999999999</v>
+      </c>
+      <c r="BJ8">
+        <v>1.0254037</v>
+      </c>
+      <c r="BK8">
+        <v>1</v>
+      </c>
+      <c r="BL8">
+        <v>0.18963360000000001</v>
+      </c>
+      <c r="BM8">
+        <v>93.720445999999995</v>
+      </c>
+      <c r="BN8">
+        <v>1.24722</v>
+      </c>
+      <c r="BO8">
+        <v>892.13088000000005</v>
+      </c>
+      <c r="BP8">
+        <v>253.95389</v>
+      </c>
+      <c r="BQ8">
+        <v>16.366099999999999</v>
+      </c>
+      <c r="BR8">
+        <v>1594.0009</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add gitlabhq to distributions
</commit_message>
<xml_diff>
--- a/data/distributions.xlsx
+++ b/data/distributions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="5180" windowWidth="21340" windowHeight="11880" tabRatio="500"/>
+    <workbookView xWindow="7320" yWindow="4740" windowWidth="21340" windowHeight="11880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all branch segments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
   <si>
     <t>repository</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>git</t>
+  </si>
+  <si>
+    <t>gitlabhq</t>
   </si>
 </sst>
 </file>
@@ -313,9 +316,101 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="618">
+  <cellStyleXfs count="710">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -938,7 +1033,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="618">
+  <cellStyles count="710">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1247,6 +1342,52 @@
     <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="697" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="699" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="701" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1555,6 +1696,52 @@
     <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="624" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="626" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="628" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="630" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="632" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="634" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="650" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="652" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="654" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="656" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="668" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="670" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="672" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="674" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="676" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="696" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="698" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="700" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="702" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1885,10 +2072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL8"/>
+  <dimension ref="A1:BL9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3511,6 +3698,200 @@
         <v>1131.3163784000001</v>
       </c>
     </row>
+    <row r="9" spans="1:64">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9">
+        <v>2.0412639404999999</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2.7487880141000001</v>
+      </c>
+      <c r="E9">
+        <v>6.2832713755</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>26.634388443999999</v>
+      </c>
+      <c r="H9">
+        <v>2.967127922</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>9.7612402215999996</v>
+      </c>
+      <c r="K9">
+        <v>6.3434944238000002</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>26.780841359</v>
+      </c>
+      <c r="N9">
+        <v>2.9755332358</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>9.7650727133000004</v>
+      </c>
+      <c r="Q9">
+        <v>119.84628253</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
+      </c>
+      <c r="S9">
+        <v>2818.3161455999998</v>
+      </c>
+      <c r="T9">
+        <v>94.158178438999997</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <v>2803.6495721000001</v>
+      </c>
+      <c r="W9">
+        <v>214.00446097</v>
+      </c>
+      <c r="X9">
+        <v>13</v>
+      </c>
+      <c r="Y9">
+        <v>4318.0012122999997</v>
+      </c>
+      <c r="Z9">
+        <v>77.947859895999997</v>
+      </c>
+      <c r="AA9">
+        <v>10</v>
+      </c>
+      <c r="AB9">
+        <v>2258.2000170000001</v>
+      </c>
+      <c r="AC9">
+        <v>133.96914498000001</v>
+      </c>
+      <c r="AD9">
+        <v>8</v>
+      </c>
+      <c r="AE9">
+        <v>2921.9559586999999</v>
+      </c>
+      <c r="AF9">
+        <v>108.28104089</v>
+      </c>
+      <c r="AG9">
+        <v>4</v>
+      </c>
+      <c r="AH9">
+        <v>2903.5267401999999</v>
+      </c>
+      <c r="AI9">
+        <v>242.25018587</v>
+      </c>
+      <c r="AJ9">
+        <v>14</v>
+      </c>
+      <c r="AK9">
+        <v>4579.8481570000004</v>
+      </c>
+      <c r="AL9">
+        <v>86.151218768999996</v>
+      </c>
+      <c r="AM9">
+        <v>10</v>
+      </c>
+      <c r="AN9">
+        <v>2313.5980109000002</v>
+      </c>
+      <c r="AO9">
+        <v>12.09535316</v>
+      </c>
+      <c r="AP9">
+        <v>3</v>
+      </c>
+      <c r="AQ9">
+        <v>45.567329295999997</v>
+      </c>
+      <c r="AR9">
+        <v>5.7181297797999999</v>
+      </c>
+      <c r="AS9">
+        <v>2</v>
+      </c>
+      <c r="AT9">
+        <v>22.544356558</v>
+      </c>
+      <c r="AU9">
+        <v>13.909665428</v>
+      </c>
+      <c r="AV9">
+        <v>3</v>
+      </c>
+      <c r="AW9">
+        <v>51.091688951999998</v>
+      </c>
+      <c r="AX9">
+        <v>6.0126516023000001</v>
+      </c>
+      <c r="AY9">
+        <v>2.5</v>
+      </c>
+      <c r="AZ9">
+        <v>22.645792496999999</v>
+      </c>
+      <c r="BA9">
+        <v>1.0416356876999999</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
+      </c>
+      <c r="BC9">
+        <v>0.23721191699999999</v>
+      </c>
+      <c r="BD9">
+        <v>1.0271375465000001</v>
+      </c>
+      <c r="BE9">
+        <v>1</v>
+      </c>
+      <c r="BF9">
+        <v>0.18090573709999999</v>
+      </c>
+      <c r="BG9">
+        <v>8.6295730587000001</v>
+      </c>
+      <c r="BH9">
+        <v>0</v>
+      </c>
+      <c r="BI9">
+        <v>82.101421805000001</v>
+      </c>
+      <c r="BJ9">
+        <v>22.191566760000001</v>
+      </c>
+      <c r="BK9">
+        <v>0</v>
+      </c>
+      <c r="BL9">
+        <v>204.53741314000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3524,10 +3905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR8"/>
+  <dimension ref="A1:BR9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5321,6 +5702,221 @@
         <v>1594.0009</v>
       </c>
     </row>
+    <row r="9" spans="1:70">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9">
+        <v>5380</v>
+      </c>
+      <c r="C9">
+        <v>10982</v>
+      </c>
+      <c r="D9">
+        <f>B9-3569</f>
+        <v>1811</v>
+      </c>
+      <c r="E9">
+        <v>7413</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33661710037174719</v>
+      </c>
+      <c r="G9" s="1">
+        <f>E9/C9</f>
+        <v>0.67501365871425967</v>
+      </c>
+      <c r="H9">
+        <v>4.0933185999999999</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>4.0129093999999998</v>
+      </c>
+      <c r="K9">
+        <v>13.049696000000001</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>43.405256999999999</v>
+      </c>
+      <c r="N9">
+        <v>3.1983149000000002</v>
+      </c>
+      <c r="O9">
+        <v>1.6666700000000001</v>
+      </c>
+      <c r="P9">
+        <v>11.312279</v>
+      </c>
+      <c r="Q9">
+        <v>13.228603</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>43.644250999999997</v>
+      </c>
+      <c r="T9">
+        <v>3.2232848000000001</v>
+      </c>
+      <c r="U9">
+        <v>1.6666700000000001</v>
+      </c>
+      <c r="V9">
+        <v>11.321576</v>
+      </c>
+      <c r="W9">
+        <v>310.28602999999998</v>
+      </c>
+      <c r="X9">
+        <v>42</v>
+      </c>
+      <c r="Y9">
+        <v>4844.6867000000002</v>
+      </c>
+      <c r="Z9">
+        <v>170.29706999999999</v>
+      </c>
+      <c r="AA9">
+        <v>15</v>
+      </c>
+      <c r="AB9">
+        <v>2965.0011</v>
+      </c>
+      <c r="AC9">
+        <v>480.5831</v>
+      </c>
+      <c r="AD9">
+        <v>64</v>
+      </c>
+      <c r="AE9">
+        <v>6376.4898000000003</v>
+      </c>
+      <c r="AF9">
+        <v>76.395077999999998</v>
+      </c>
+      <c r="AG9">
+        <v>20.333300000000001</v>
+      </c>
+      <c r="AH9">
+        <v>715.17354999999998</v>
+      </c>
+      <c r="AI9">
+        <v>352.24130000000002</v>
+      </c>
+      <c r="AJ9">
+        <v>44</v>
+      </c>
+      <c r="AK9">
+        <v>5022.1342000000004</v>
+      </c>
+      <c r="AL9">
+        <v>212.25235000000001</v>
+      </c>
+      <c r="AM9">
+        <v>19</v>
+      </c>
+      <c r="AN9">
+        <v>3236.9213</v>
+      </c>
+      <c r="AO9">
+        <v>564.49365</v>
+      </c>
+      <c r="AP9">
+        <v>71</v>
+      </c>
+      <c r="AQ9">
+        <v>6894.5023000000001</v>
+      </c>
+      <c r="AR9">
+        <v>100.76508</v>
+      </c>
+      <c r="AS9">
+        <v>22</v>
+      </c>
+      <c r="AT9">
+        <v>1124.1992</v>
+      </c>
+      <c r="AU9">
+        <v>24.886803</v>
+      </c>
+      <c r="AV9">
+        <v>11</v>
+      </c>
+      <c r="AW9">
+        <v>68.838284000000002</v>
+      </c>
+      <c r="AX9">
+        <v>5.9417660000000003</v>
+      </c>
+      <c r="AY9">
+        <v>3.2727300000000001</v>
+      </c>
+      <c r="AZ9">
+        <v>18.033339000000002</v>
+      </c>
+      <c r="BA9">
+        <v>30.276643</v>
+      </c>
+      <c r="BB9">
+        <v>13</v>
+      </c>
+      <c r="BC9">
+        <v>78.538875000000004</v>
+      </c>
+      <c r="BD9">
+        <v>6.8167121000000002</v>
+      </c>
+      <c r="BE9">
+        <v>4</v>
+      </c>
+      <c r="BF9">
+        <v>18.382714</v>
+      </c>
+      <c r="BG9">
+        <v>1.1236885999999999</v>
+      </c>
+      <c r="BH9">
+        <v>1</v>
+      </c>
+      <c r="BI9">
+        <v>0.39631850000000002</v>
+      </c>
+      <c r="BJ9">
+        <v>1.0806184000000001</v>
+      </c>
+      <c r="BK9">
+        <v>1</v>
+      </c>
+      <c r="BL9">
+        <v>0.30486819999999998</v>
+      </c>
+      <c r="BM9">
+        <v>25.63617</v>
+      </c>
+      <c r="BN9">
+        <v>1.4313899999999999</v>
+      </c>
+      <c r="BO9">
+        <v>139.98491000000001</v>
+      </c>
+      <c r="BP9">
+        <v>65.925251000000003</v>
+      </c>
+      <c r="BQ9">
+        <v>2.3675000000000002</v>
+      </c>
+      <c r="BR9">
+        <v>348.48689999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add godot to distributions
</commit_message>
<xml_diff>
--- a/data/distributions.xlsx
+++ b/data/distributions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
   <si>
     <t>repository</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>gitlabhq</t>
+  </si>
+  <si>
+    <t>godot</t>
   </si>
 </sst>
 </file>
@@ -316,9 +319,97 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="710">
+  <cellStyleXfs count="798">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1033,7 +1124,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="710">
+  <cellStyles count="798">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1388,6 +1479,50 @@
     <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="777" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1742,6 +1877,50 @@
     <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="710" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="712" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="714" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="716" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="718" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="720" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="738" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="740" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="742" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="750" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="772" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="774" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="776" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2072,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL9"/>
+  <dimension ref="A1:BL10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3892,6 +4071,200 @@
         <v>204.53741314000001</v>
       </c>
     </row>
+    <row r="10" spans="1:64">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>1.5248756218999999</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1.2596275068</v>
+      </c>
+      <c r="E10">
+        <v>26.654228856</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>184.99715531999999</v>
+      </c>
+      <c r="H10">
+        <v>14.650171759999999</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>82.991788528000001</v>
+      </c>
+      <c r="K10">
+        <v>26.661691542</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>184.99639404999999</v>
+      </c>
+      <c r="N10">
+        <v>14.653156835000001</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>82.991389424999994</v>
+      </c>
+      <c r="Q10">
+        <v>5944.0547263999997</v>
+      </c>
+      <c r="R10">
+        <v>14</v>
+      </c>
+      <c r="S10">
+        <v>69590.731713000001</v>
+      </c>
+      <c r="T10">
+        <v>1479.9353234</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+      <c r="V10">
+        <v>12219.597841999999</v>
+      </c>
+      <c r="W10">
+        <v>7423.9900497999997</v>
+      </c>
+      <c r="X10">
+        <v>22</v>
+      </c>
+      <c r="Y10">
+        <v>71764.104538</v>
+      </c>
+      <c r="Z10">
+        <v>4231.8666855000001</v>
+      </c>
+      <c r="AA10">
+        <v>16.7</v>
+      </c>
+      <c r="AB10">
+        <v>32838.154939</v>
+      </c>
+      <c r="AC10">
+        <v>5946.4651740999998</v>
+      </c>
+      <c r="AD10">
+        <v>14</v>
+      </c>
+      <c r="AE10">
+        <v>69590.661124999999</v>
+      </c>
+      <c r="AF10">
+        <v>1482.3457711000001</v>
+      </c>
+      <c r="AG10">
+        <v>4</v>
+      </c>
+      <c r="AH10">
+        <v>12219.431757</v>
+      </c>
+      <c r="AI10">
+        <v>7428.8109452999997</v>
+      </c>
+      <c r="AJ10">
+        <v>22</v>
+      </c>
+      <c r="AK10">
+        <v>71763.911078000005</v>
+      </c>
+      <c r="AL10">
+        <v>4233.1761532999999</v>
+      </c>
+      <c r="AM10">
+        <v>18.125</v>
+      </c>
+      <c r="AN10">
+        <v>32838.041462000001</v>
+      </c>
+      <c r="AO10">
+        <v>166.79104477999999</v>
+      </c>
+      <c r="AP10">
+        <v>4</v>
+      </c>
+      <c r="AQ10">
+        <v>1350.506079</v>
+      </c>
+      <c r="AR10">
+        <v>147.37474101000001</v>
+      </c>
+      <c r="AS10">
+        <v>3.6</v>
+      </c>
+      <c r="AT10">
+        <v>1344.4942458</v>
+      </c>
+      <c r="AU10">
+        <v>168.67910448000001</v>
+      </c>
+      <c r="AV10">
+        <v>5</v>
+      </c>
+      <c r="AW10">
+        <v>1350.4747789999999</v>
+      </c>
+      <c r="AX10">
+        <v>147.82556536000001</v>
+      </c>
+      <c r="AY10">
+        <v>4</v>
+      </c>
+      <c r="AZ10">
+        <v>1344.4606898</v>
+      </c>
+      <c r="BA10">
+        <v>1.0124378109000001</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
+      <c r="BC10">
+        <v>0.110967306</v>
+      </c>
+      <c r="BD10">
+        <v>1.0074626866</v>
+      </c>
+      <c r="BE10">
+        <v>1</v>
+      </c>
+      <c r="BF10">
+        <v>8.6171144699999994E-2</v>
+      </c>
+      <c r="BG10">
+        <v>13.324094804</v>
+      </c>
+      <c r="BH10">
+        <v>0</v>
+      </c>
+      <c r="BI10">
+        <v>79.288798958000001</v>
+      </c>
+      <c r="BJ10">
+        <v>19.814127280000001</v>
+      </c>
+      <c r="BK10">
+        <v>0</v>
+      </c>
+      <c r="BL10">
+        <v>159.85899377000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3905,10 +4278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR9"/>
+  <dimension ref="A1:BR10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5917,6 +6290,221 @@
         <v>348.48689999999999</v>
       </c>
     </row>
+    <row r="10" spans="1:70">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>402</v>
+      </c>
+      <c r="C10">
+        <v>613</v>
+      </c>
+      <c r="D10">
+        <f>B10-301</f>
+        <v>101</v>
+      </c>
+      <c r="E10">
+        <v>311</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25124378109452739</v>
+      </c>
+      <c r="G10" s="1">
+        <f>E10/C10</f>
+        <v>0.5073409461663948</v>
+      </c>
+      <c r="H10">
+        <v>3.11</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>1.7459621999999999</v>
+      </c>
+      <c r="K10">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="L10">
+        <v>5.5</v>
+      </c>
+      <c r="M10">
+        <v>340.01175999999998</v>
+      </c>
+      <c r="N10">
+        <v>20.143689999999999</v>
+      </c>
+      <c r="O10">
+        <v>1.6666700000000001</v>
+      </c>
+      <c r="P10">
+        <v>84.762940999999998</v>
+      </c>
+      <c r="Q10">
+        <v>68.430000000000007</v>
+      </c>
+      <c r="R10">
+        <v>5.5</v>
+      </c>
+      <c r="S10">
+        <v>340.00637</v>
+      </c>
+      <c r="T10">
+        <v>20.15569</v>
+      </c>
+      <c r="U10">
+        <v>1.6667000000000001</v>
+      </c>
+      <c r="V10">
+        <v>84.760571999999996</v>
+      </c>
+      <c r="W10">
+        <v>14432.54</v>
+      </c>
+      <c r="X10">
+        <v>172.5</v>
+      </c>
+      <c r="Y10">
+        <v>129590.84</v>
+      </c>
+      <c r="Z10">
+        <v>2002.15</v>
+      </c>
+      <c r="AA10">
+        <v>25.5</v>
+      </c>
+      <c r="AB10">
+        <v>11109.769</v>
+      </c>
+      <c r="AC10">
+        <v>16434.689999999999</v>
+      </c>
+      <c r="AD10">
+        <v>253</v>
+      </c>
+      <c r="AE10">
+        <v>129944.67</v>
+      </c>
+      <c r="AF10">
+        <v>3602.3541</v>
+      </c>
+      <c r="AG10">
+        <v>69.5</v>
+      </c>
+      <c r="AH10">
+        <v>22397.338</v>
+      </c>
+      <c r="AI10">
+        <v>14442.23</v>
+      </c>
+      <c r="AJ10">
+        <v>175</v>
+      </c>
+      <c r="AK10">
+        <v>129590.05</v>
+      </c>
+      <c r="AL10">
+        <v>2011.84</v>
+      </c>
+      <c r="AM10">
+        <v>34.5</v>
+      </c>
+      <c r="AN10">
+        <v>11108.566000000001</v>
+      </c>
+      <c r="AO10">
+        <v>16454.07</v>
+      </c>
+      <c r="AP10">
+        <v>266</v>
+      </c>
+      <c r="AQ10">
+        <v>129942.88</v>
+      </c>
+      <c r="AR10">
+        <v>3607.6181000000001</v>
+      </c>
+      <c r="AS10">
+        <v>73.75</v>
+      </c>
+      <c r="AT10">
+        <v>22396.812999999998</v>
+      </c>
+      <c r="AU10">
+        <v>114.42</v>
+      </c>
+      <c r="AV10">
+        <v>22.5</v>
+      </c>
+      <c r="AW10">
+        <v>289.44914999999997</v>
+      </c>
+      <c r="AX10">
+        <v>36.366458999999999</v>
+      </c>
+      <c r="AY10">
+        <v>7.75</v>
+      </c>
+      <c r="AZ10">
+        <v>72.621058000000005</v>
+      </c>
+      <c r="BA10">
+        <v>122.01</v>
+      </c>
+      <c r="BB10">
+        <v>31.5</v>
+      </c>
+      <c r="BC10">
+        <v>290.16838000000001</v>
+      </c>
+      <c r="BD10">
+        <v>38.178773</v>
+      </c>
+      <c r="BE10">
+        <v>9.6666699999999999</v>
+      </c>
+      <c r="BF10">
+        <v>72.885351999999997</v>
+      </c>
+      <c r="BG10">
+        <v>1.05</v>
+      </c>
+      <c r="BH10">
+        <v>1</v>
+      </c>
+      <c r="BI10">
+        <v>0.21904290000000001</v>
+      </c>
+      <c r="BJ10">
+        <v>1.03</v>
+      </c>
+      <c r="BK10">
+        <v>1</v>
+      </c>
+      <c r="BL10">
+        <v>0.1714466</v>
+      </c>
+      <c r="BM10">
+        <v>53.562860999999998</v>
+      </c>
+      <c r="BN10">
+        <v>3.1804199999999998</v>
+      </c>
+      <c r="BO10">
+        <v>152.60174000000001</v>
+      </c>
+      <c r="BP10">
+        <v>79.652792000000005</v>
+      </c>
+      <c r="BQ10">
+        <v>4.83528</v>
+      </c>
+      <c r="BR10">
+        <v>314.15884999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>